<commit_message>
Updated sprint log and added a reflection over the sprint
</commit_message>
<xml_diff>
--- a/doc/Sprint#04/Sprintplaning.xlsx
+++ b/doc/Sprint#04/Sprintplaning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Write testcases</t>
   </si>
@@ -40,6 +40,21 @@
   </si>
   <si>
     <t>40H</t>
+  </si>
+  <si>
+    <t>Extra things</t>
+  </si>
+  <si>
+    <t>Fix the button Settings</t>
+  </si>
+  <si>
+    <t>Fix the button History</t>
+  </si>
+  <si>
+    <t>Fix the button Profile</t>
+  </si>
+  <si>
+    <t>10H</t>
   </si>
 </sst>
 </file>
@@ -378,13 +393,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -416,6 +434,35 @@
       </c>
       <c r="D4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>